<commit_message>
xinyu email to CIO
</commit_message>
<xml_diff>
--- a/Database/KPIData/KPI_2025S1.xlsx
+++ b/Database/KPIData/KPI_2025S1.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <x:si>
     <x:t>Staff_ID</x:t>
   </x:si>
@@ -38,7 +38,7 @@
     <x:t>AvgComplexity</x:t>
   </x:si>
   <x:si>
-    <x:t>FirstFinalScore</x:t>
+    <x:t>FinalScore</x:t>
   </x:si>
   <x:si>
     <x:t>DI0004</x:t>
@@ -81,9 +81,6 @@
   </x:si>
   <x:si>
     <x:t>ErrorRate</x:t>
-  </x:si>
-  <x:si>
-    <x:t>SecondFinalScore</x:t>
   </x:si>
   <x:si>
     <x:t>PE0002</x:t>
@@ -617,18 +614,18 @@
         <x:v>21</x:v>
       </x:c>
       <x:c r="K1" s="0" t="s">
-        <x:v>22</x:v>
+        <x:v>7</x:v>
       </x:c>
     </x:row>
     <x:row r="2" spans="1:11">
       <x:c r="A2" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="B2" s="0" t="s">
         <x:v>23</x:v>
       </x:c>
-      <x:c r="B2" s="0" t="s">
+      <x:c r="C2" s="0" t="s">
         <x:v>24</x:v>
-      </x:c>
-      <x:c r="C2" s="0" t="s">
-        <x:v>25</x:v>
       </x:c>
       <x:c r="D2" s="0" t="n">
         <x:v>31</x:v>
@@ -657,13 +654,13 @@
     </x:row>
     <x:row r="3" spans="1:11">
       <x:c r="A3" s="0" t="s">
+        <x:v>25</x:v>
+      </x:c>
+      <x:c r="B3" s="0" t="s">
         <x:v>26</x:v>
       </x:c>
-      <x:c r="B3" s="0" t="s">
-        <x:v>27</x:v>
-      </x:c>
       <x:c r="C3" s="0" t="s">
-        <x:v>25</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="D3" s="0" t="n">
         <x:v>27</x:v>
@@ -692,13 +689,13 @@
     </x:row>
     <x:row r="4" spans="1:11">
       <x:c r="A4" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="B4" s="0" t="s">
         <x:v>23</x:v>
       </x:c>
-      <x:c r="B4" s="0" t="s">
-        <x:v>24</x:v>
-      </x:c>
       <x:c r="C4" s="0" t="s">
-        <x:v>28</x:v>
+        <x:v>27</x:v>
       </x:c>
       <x:c r="D4" s="0" t="n">
         <x:v>32</x:v>
@@ -727,13 +724,13 @@
     </x:row>
     <x:row r="5" spans="1:11">
       <x:c r="A5" s="0" t="s">
+        <x:v>25</x:v>
+      </x:c>
+      <x:c r="B5" s="0" t="s">
         <x:v>26</x:v>
       </x:c>
-      <x:c r="B5" s="0" t="s">
+      <x:c r="C5" s="0" t="s">
         <x:v>27</x:v>
-      </x:c>
-      <x:c r="C5" s="0" t="s">
-        <x:v>28</x:v>
       </x:c>
       <x:c r="D5" s="0" t="n">
         <x:v>28</x:v>
@@ -762,13 +759,13 @@
     </x:row>
     <x:row r="6" spans="1:11">
       <x:c r="A6" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="B6" s="0" t="s">
         <x:v>23</x:v>
       </x:c>
-      <x:c r="B6" s="0" t="s">
-        <x:v>24</x:v>
-      </x:c>
       <x:c r="C6" s="0" t="s">
-        <x:v>29</x:v>
+        <x:v>28</x:v>
       </x:c>
       <x:c r="D6" s="0" t="n">
         <x:v>32</x:v>
@@ -797,13 +794,13 @@
     </x:row>
     <x:row r="7" spans="1:11">
       <x:c r="A7" s="0" t="s">
+        <x:v>25</x:v>
+      </x:c>
+      <x:c r="B7" s="0" t="s">
         <x:v>26</x:v>
       </x:c>
-      <x:c r="B7" s="0" t="s">
-        <x:v>27</x:v>
-      </x:c>
       <x:c r="C7" s="0" t="s">
-        <x:v>29</x:v>
+        <x:v>28</x:v>
       </x:c>
       <x:c r="D7" s="0" t="n">
         <x:v>27</x:v>

</xml_diff>